<commit_message>
docs: remove BCNF section and align normalisation with 3NF and 4NF design
</commit_message>
<xml_diff>
--- a/docs/Medialog Normalisation.xlsx
+++ b/docs/Medialog Normalisation.xlsx
@@ -5,21 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/021ef743cc8590fc/Desktop/Course/phase 5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cjoss\Development\web-dev\dev1002-medialog\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="263" documentId="8_{1BE095B7-0242-48A8-A912-1A152EA62524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24DA1801-7B74-4BDB-9570-F9719A0BA2EC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7041454-E83D-484B-AAA3-14209E16D033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="30960" windowHeight="12120" activeTab="5" xr2:uid="{7130AD04-D86D-4F77-8531-7D31C2FCAB0B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{7130AD04-D86D-4F77-8531-7D31C2FCAB0B}"/>
   </bookViews>
   <sheets>
     <sheet name="UNF" sheetId="1" r:id="rId1"/>
     <sheet name="1NF" sheetId="2" r:id="rId2"/>
     <sheet name="2NF" sheetId="3" r:id="rId3"/>
     <sheet name="3NF" sheetId="4" r:id="rId4"/>
-    <sheet name="BCNF" sheetId="6" r:id="rId5"/>
-    <sheet name="4NF" sheetId="7" r:id="rId6"/>
-    <sheet name="Summary" sheetId="5" r:id="rId7"/>
+    <sheet name="4NF" sheetId="7" r:id="rId5"/>
+    <sheet name="Summary" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="70">
   <si>
     <t>user_id</t>
   </si>
@@ -200,24 +199,12 @@
     <t>(item_id, creator_id)</t>
   </si>
   <si>
-    <t>3NF to BCNF</t>
-  </si>
-  <si>
-    <t>BCNF to 4NF</t>
-  </si>
-  <si>
     <t>Eliminates partial dependencies; each non-key depends on the whole key.</t>
   </si>
   <si>
     <t>Ensures atomic values (each cell holds a single value).</t>
   </si>
   <si>
-    <t>Every determinant is a candidate key; resolves user–item dependency.</t>
-  </si>
-  <si>
-    <t>Removes nontrivial multivalued dependencies; prevents redundancy.</t>
-  </si>
-  <si>
     <t>Split repeating lists (tag_list, creator_list) into individual rows</t>
   </si>
   <si>
@@ -230,12 +217,6 @@
     <t xml:space="preserve">Confirms all non-key attributes depend only on the primary key. </t>
   </si>
   <si>
-    <t>Moved user-specific rating/review to Review(user_id, item_id, …)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Added item_tags and item_creators join tables for independent MVDs </t>
-  </si>
-  <si>
     <t>Note: No structural changes. All non-key attributes depend solely on the primary key.</t>
   </si>
   <si>
@@ -261,6 +242,15 @@
   </si>
   <si>
     <t>item_creators (Items &lt;-&gt; Creators)</t>
+  </si>
+  <si>
+    <t>3NF to 4NF (design)</t>
+  </si>
+  <si>
+    <t>Used item_tags and item_creators junction tables to store multi-valued sets</t>
+  </si>
+  <si>
+    <t>Removes multi-valued dependencies and prevents repeating tag/creator values in the Item table.</t>
   </si>
 </sst>
 </file>
@@ -376,10 +366,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -701,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E597D8A-76E2-4F15-A179-C9271BB7019B}">
   <dimension ref="B2:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -787,25 +773,25 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I4" s="1">
         <v>4</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -971,7 +957,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>15</v>
@@ -980,16 +966,16 @@
         <v>18</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I6" s="1">
         <v>4</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1003,7 +989,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>15</v>
@@ -1012,16 +998,16 @@
         <v>20</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I7" s="1">
         <v>4</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1035,25 +1021,25 @@
         <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I8" s="1">
         <v>4</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1190,7 +1176,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>47</v>
@@ -1252,13 +1238,13 @@
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
@@ -1321,7 +1307,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
@@ -1354,7 +1340,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1491,7 +1477,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>47</v>
@@ -1553,13 +1539,13 @@
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D22" s="1">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
@@ -1622,7 +1608,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
@@ -1655,12 +1641,12 @@
         <v>2</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1670,310 +1656,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D6EB769-97D8-4C68-AF28-01754D16111A}">
-  <dimension ref="B2:G37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="4" width="19.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="B2" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="7" spans="2:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
-        <v>2</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="13" spans="2:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="B13" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="1">
-        <v>10</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="1">
-        <v>11</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="1">
-        <v>2</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="2:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1">
-        <v>10</v>
-      </c>
-      <c r="D21" s="1">
-        <v>5</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1">
-        <v>11</v>
-      </c>
-      <c r="D22" s="1">
-        <v>4</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-    </row>
-    <row r="25" spans="2:6" ht="18" x14ac:dyDescent="0.3">
-      <c r="B25" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="1">
-        <v>1</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="1">
-        <v>2</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="1">
-        <v>3</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="1">
-        <v>4</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="1">
-        <v>5</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="34" spans="2:3" ht="18" x14ac:dyDescent="0.3">
-      <c r="B34" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="1">
-        <v>1</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B37" s="1">
-        <v>2</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78D8BF02-6D19-4A93-9A56-F3DC1C661F0D}">
   <dimension ref="B2:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S45" sqref="S45"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2085,13 +1772,13 @@
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D16" s="1">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F16" s="1">
         <v>1</v>
@@ -2161,7 +1848,7 @@
         <v>4</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>47</v>
@@ -2224,7 +1911,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
@@ -2257,12 +1944,12 @@
         <v>2</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="18" x14ac:dyDescent="0.3">
       <c r="B40" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
@@ -2338,7 +2025,7 @@
     </row>
     <row r="49" spans="2:4" ht="18" x14ac:dyDescent="0.3">
       <c r="B49" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
@@ -2380,12 +2067,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC34CB3E-D765-4163-A4D4-A184F22160D9}">
-  <dimension ref="B2:D7"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D16" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2412,10 +2099,10 @@
         <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
@@ -2423,10 +2110,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
@@ -2434,32 +2121,21 @@
         <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>